<commit_message>
Added filtered version of man_data, that only contains data for "complete" hours
</commit_message>
<xml_diff>
--- a/01_Input/Manual_Counts/013_08.12.2023 (MaVI13).xlsx
+++ b/01_Input/Manual_Counts/013_08.12.2023 (MaVI13).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailunimannheimde-my.sharepoint.com/personal/pstapf_mail_uni-mannheim_de/Documents/Uni/Master/Semester 3/Teamproject/Towards-Sustainable-Cities-through-Simulation/01_Input/Manual_Counts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_AD4DB114E441178AC67DF4B50ED1E6EA693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20138555-1329-42EE-B0B0-8E931C439D32}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_AD4DB114E441178AC67DF4B50ED1E6EA693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87728654-FFA2-425A-ABAF-97EFC6435251}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,6 +425,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>